<commit_message>
DMS: Translate Export Template Eroute
</commit_message>
<xml_diff>
--- a/DMS/Templates/ERoute_Template.xlsx
+++ b/DMS/Templates/ERoute_Template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496F31F2-A3C8-4290-8D47-2F0BB1B46F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468B8EF0-1336-4CD6-A557-14A8F6CF3E07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ERoute" sheetId="1" r:id="rId1"/>
+    <sheet name="Tuyến" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>